<commit_message>
resolve the mainGragh problem
</commit_message>
<xml_diff>
--- a/static/excelsFiles/excelPerAge.xlsx
+++ b/static/excelsFiles/excelPerAge.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara\Desktop\it\python\semester b\small-project-Python-use-OpenCV-Flask-DB\excelsFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara\Desktop\it\python\semester b\small-project-Python-use-OpenCV-Flask-DB\static\excelsFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7D26BA-5C2E-4E37-9516-B4713C25886C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED15396-CA48-48F8-8512-4E59B4696222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,13 +54,13 @@
     <t>"50-100"</t>
   </si>
   <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>famale</t>
-  </si>
-  <si>
     <t>child</t>
+  </si>
+  <si>
+    <t>man</t>
+  </si>
+  <si>
+    <t>woman</t>
   </si>
 </sst>
 </file>
@@ -422,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -433,13 +433,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -523,7 +523,7 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -537,7 +537,7 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -551,7 +551,7 @@
         <v>3</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>